<commit_message>
Reran RF plan with cross validation
</commit_message>
<xml_diff>
--- a/Analysis/Multivariate/Summary/candidates_summary_19042023.xlsx
+++ b/Analysis/Multivariate/Summary/candidates_summary_19042023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chrismbrooks/Documents/Imperial/Asquith Group/KIR_HLA/Analysis/Multivariate/Summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2C6C051-BD98-EF47-94F2-CBFBF8685364}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD8D5C42-E165-1547-8FE0-7F210F6AEFE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10080" yWindow="3260" windowWidth="26800" windowHeight="16580" xr2:uid="{A6591B52-7433-0C47-834F-419CD579EE68}"/>
+    <workbookView xWindow="9040" yWindow="3260" windowWidth="26800" windowHeight="16580" xr2:uid="{A6591B52-7433-0C47-834F-419CD579EE68}"/>
   </bookViews>
   <sheets>
     <sheet name="Robustness Summary" sheetId="1" r:id="rId1"/>
@@ -257,9 +257,6 @@
     <t>Run ID</t>
   </si>
   <si>
-    <t>tt Score (neg mae)</t>
-  </si>
-  <si>
     <t>07042023</t>
   </si>
   <si>
@@ -324,6 +321,9 @@
   </si>
   <si>
     <t>importance_mean_2</t>
+  </si>
+  <si>
+    <t>EN tt Score (neg mae)</t>
   </si>
 </sst>
 </file>
@@ -394,7 +394,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -413,7 +413,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -735,7 +734,7 @@
   <dimension ref="B4:M24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -744,7 +743,7 @@
     <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="20.1640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.5" bestFit="1" customWidth="1"/>
@@ -772,13 +771,13 @@
         <v>9</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="I4" s="9" t="s">
         <v>62</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K4" s="9" t="s">
         <v>62</v>
@@ -814,7 +813,7 @@
         <v>-0.22076642799999999</v>
       </c>
       <c r="K5" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.2">
@@ -844,10 +843,10 @@
         <v>1.2675418741512108E-2</v>
       </c>
       <c r="J6" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K6" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.2">
@@ -877,10 +876,10 @@
         <v>1.2675418741512108E-2</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K7" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.2">
@@ -910,10 +909,10 @@
         <v>1.4033499320959797E-2</v>
       </c>
       <c r="J8" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K8" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.2">
@@ -1011,15 +1010,15 @@
         <v>1.6296966953372655E-2</v>
       </c>
       <c r="J11" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K11" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>60</v>
@@ -1112,10 +1111,10 @@
         <v>1.6296966953372655E-2</v>
       </c>
       <c r="J14" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K14" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.2">
@@ -1383,7 +1382,7 @@
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B24" s="2" t="str">
-        <v>tt Score (neg mae)</v>
+        <v>EN tt Score (neg mae)</v>
       </c>
       <c r="C24" s="2">
         <v>-0.22090000000000001</v>
@@ -1446,25 +1445,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" t="s">
         <v>83</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>84</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>85</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>86</v>
       </c>
-      <c r="E1" t="s">
-        <v>87</v>
-      </c>
       <c r="F1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G1" t="s">
         <v>74</v>
-      </c>
-      <c r="G1" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -1477,16 +1476,16 @@
       <c r="C2" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="12">
+      <c r="D2" s="11">
         <v>2.1866480158678699E-2</v>
       </c>
-      <c r="E2" s="12">
+      <c r="E2" s="11">
         <v>1.37840434008098E-2</v>
       </c>
-      <c r="F2" s="12">
+      <c r="F2" s="11">
         <v>3.5650523559488501E-2</v>
       </c>
-      <c r="G2" s="13">
+      <c r="G2" s="12">
         <v>1</v>
       </c>
     </row>
@@ -1500,16 +1499,16 @@
       <c r="C3" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="12">
+      <c r="D3" s="11">
         <v>1.03901108566565E-2</v>
       </c>
-      <c r="E3" s="12">
+      <c r="E3" s="11">
         <v>1.8165863962514E-2</v>
       </c>
-      <c r="F3" s="12">
+      <c r="F3" s="11">
         <v>2.85559748191705E-2</v>
       </c>
-      <c r="G3" s="13">
+      <c r="G3" s="12">
         <v>0.80099734780950305</v>
       </c>
     </row>
@@ -1523,39 +1522,39 @@
       <c r="C4" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="11">
         <v>1.18692470491119E-2</v>
       </c>
-      <c r="E4" s="12">
+      <c r="E4" s="11">
         <v>8.8774876311529007E-3</v>
       </c>
-      <c r="F4" s="12">
+      <c r="F4" s="11">
         <v>2.0746734680264799E-2</v>
       </c>
-      <c r="G4" s="13">
+      <c r="G4" s="12">
         <v>0.58194754547280603</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" t="s">
         <v>76</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>77</v>
       </c>
-      <c r="C5" t="s">
-        <v>78</v>
-      </c>
-      <c r="D5" s="12">
+      <c r="D5" s="11">
         <v>1.21156011075578E-2</v>
       </c>
-      <c r="E5" s="12">
+      <c r="E5" s="11">
         <v>7.7990328220791999E-3</v>
       </c>
-      <c r="F5" s="12">
+      <c r="F5" s="11">
         <v>1.9914633929637E-2</v>
       </c>
-      <c r="G5" s="13">
+      <c r="G5" s="12">
         <v>0.55860705373390396</v>
       </c>
     </row>
@@ -1569,16 +1568,16 @@
       <c r="C6" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="12">
+      <c r="D6" s="11">
         <v>1.1781234134518301E-2</v>
       </c>
-      <c r="E6" s="12">
+      <c r="E6" s="11">
         <v>1.2136333120779999E-3</v>
       </c>
-      <c r="F6" s="12">
+      <c r="F6" s="11">
         <v>1.29948674465963E-2</v>
       </c>
-      <c r="G6" s="13">
+      <c r="G6" s="12">
         <v>0.36450705765687602</v>
       </c>
     </row>
@@ -1592,16 +1591,16 @@
       <c r="C7" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="11">
         <v>1.03665909710696E-2</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="11">
         <v>1.6077873022027E-3</v>
       </c>
-      <c r="F7" s="12">
+      <c r="F7" s="11">
         <v>1.19743782732723E-2</v>
       </c>
-      <c r="G7" s="13">
+      <c r="G7" s="12">
         <v>0.33588225579046999</v>
       </c>
     </row>
@@ -1615,16 +1614,16 @@
       <c r="C8" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="12">
+      <c r="D8" s="11">
         <v>2.6897828181806E-3</v>
       </c>
-      <c r="E8" s="12">
+      <c r="E8" s="11">
         <v>9.0456727916603998E-3</v>
       </c>
-      <c r="F8" s="12">
+      <c r="F8" s="11">
         <v>1.1735455609840999E-2</v>
       </c>
-      <c r="G8" s="13">
+      <c r="G8" s="12">
         <v>0.32918045622130998</v>
       </c>
     </row>
@@ -1638,16 +1637,16 @@
       <c r="C9" t="s">
         <v>35</v>
       </c>
-      <c r="D9" s="12">
+      <c r="D9" s="11">
         <v>6.9268326991133999E-3</v>
       </c>
-      <c r="E9" s="12">
+      <c r="E9" s="11">
         <v>3.2335035392368999E-3</v>
       </c>
-      <c r="F9" s="12">
+      <c r="F9" s="11">
         <v>1.01603362383503E-2</v>
       </c>
-      <c r="G9" s="13">
+      <c r="G9" s="12">
         <v>0.284998233515313</v>
       </c>
     </row>
@@ -1661,39 +1660,39 @@
       <c r="C10" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="12">
+      <c r="D10" s="11">
         <v>7.3216528083481997E-3</v>
       </c>
-      <c r="E10" s="12">
+      <c r="E10" s="11">
         <v>7.645211237504E-4</v>
       </c>
-      <c r="F10" s="12">
+      <c r="F10" s="11">
         <v>8.0861739320986E-3</v>
       </c>
-      <c r="G10" s="13">
+      <c r="G10" s="12">
         <v>0.226817817096165</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>78</v>
+      </c>
+      <c r="B11" t="s">
         <v>79</v>
-      </c>
-      <c r="B11" t="s">
-        <v>80</v>
       </c>
       <c r="C11" t="s">
         <v>49</v>
       </c>
-      <c r="D11" s="12">
+      <c r="D11" s="11">
         <v>7.3203303553300003E-4</v>
       </c>
-      <c r="E11" s="12">
+      <c r="E11" s="11">
         <v>6.2231287821423002E-3</v>
       </c>
-      <c r="F11" s="12">
+      <c r="F11" s="11">
         <v>6.9551618176753004E-3</v>
       </c>
-      <c r="G11" s="13">
+      <c r="G11" s="12">
         <v>0.19509283800753999</v>
       </c>
     </row>
@@ -1707,39 +1706,39 @@
       <c r="C12" t="s">
         <v>48</v>
       </c>
-      <c r="D12" s="12">
+      <c r="D12" s="11">
         <v>6.5262832233468002E-3</v>
       </c>
-      <c r="E12" s="12">
+      <c r="E12" s="11">
         <v>3.7984362484059998E-4</v>
       </c>
-      <c r="F12" s="12">
+      <c r="F12" s="11">
         <v>6.9061268481873999E-3</v>
       </c>
-      <c r="G12" s="13">
+      <c r="G12" s="12">
         <v>0.193717403242716</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>80</v>
+      </c>
+      <c r="B13" t="s">
         <v>81</v>
-      </c>
-      <c r="B13" t="s">
-        <v>82</v>
       </c>
       <c r="C13" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="12">
+      <c r="D13" s="11">
         <v>3.2342217042755001E-3</v>
       </c>
-      <c r="E13" s="12">
+      <c r="E13" s="11">
         <v>2.7235813200457999E-3</v>
       </c>
-      <c r="F13" s="12">
+      <c r="F13" s="11">
         <v>5.95780302432129E-3</v>
       </c>
-      <c r="G13" s="13">
+      <c r="G13" s="12">
         <v>0.16711684512514199</v>
       </c>
     </row>
@@ -1753,16 +1752,16 @@
       <c r="C14" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="12">
+      <c r="D14" s="11">
         <v>3.8230323616268999E-3</v>
       </c>
-      <c r="E14" s="12">
+      <c r="E14" s="11">
         <v>1.2854370302372001E-3</v>
       </c>
-      <c r="F14" s="12">
+      <c r="F14" s="11">
         <v>5.1084693918641002E-3</v>
       </c>
-      <c r="G14" s="13">
+      <c r="G14" s="12">
         <v>0.14329296969060801</v>
       </c>
     </row>
@@ -1776,16 +1775,16 @@
       <c r="C15" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="12">
+      <c r="D15" s="11">
         <v>7.9938446540126998E-3</v>
       </c>
-      <c r="E15" s="12">
+      <c r="E15" s="11">
         <v>-3.0893799672008998E-3</v>
       </c>
-      <c r="F15" s="12">
+      <c r="F15" s="11">
         <v>4.9044646868118E-3</v>
       </c>
-      <c r="G15" s="13">
+      <c r="G15" s="12">
         <v>0.137570621610309</v>
       </c>
     </row>
@@ -1799,16 +1798,16 @@
       <c r="C16" t="s">
         <v>38</v>
       </c>
-      <c r="D16" s="12">
+      <c r="D16" s="11">
         <v>9.4930903120700005E-4</v>
       </c>
-      <c r="E16" s="12">
+      <c r="E16" s="11">
         <v>1.325755983275E-4</v>
       </c>
-      <c r="F16" s="12">
+      <c r="F16" s="11">
         <v>1.0818846295345E-3</v>
       </c>
-      <c r="G16" s="13">
+      <c r="G16" s="12">
         <v>3.0346949259502601E-2</v>
       </c>
     </row>
@@ -1822,16 +1821,16 @@
       <c r="C17" t="s">
         <v>45</v>
       </c>
-      <c r="D17" s="12">
+      <c r="D17" s="11">
         <v>2.4488227651418E-3</v>
       </c>
-      <c r="E17" s="12">
+      <c r="E17" s="11">
         <v>-1.8189618431337E-3</v>
       </c>
-      <c r="F17" s="12">
+      <c r="F17" s="11">
         <v>6.2986092200809996E-4</v>
       </c>
-      <c r="G17" s="13">
+      <c r="G17" s="12">
         <v>1.7667648581852598E-2</v>
       </c>
     </row>
@@ -1845,16 +1844,16 @@
       <c r="C18" t="s">
         <v>35</v>
       </c>
-      <c r="D18" s="12">
+      <c r="D18" s="11">
         <v>0</v>
       </c>
-      <c r="E18" s="12">
+      <c r="E18" s="11">
         <v>2.955973717352E-4</v>
       </c>
-      <c r="F18" s="12">
+      <c r="F18" s="11">
         <v>2.955973717352E-4</v>
       </c>
-      <c r="G18" s="13">
+      <c r="G18" s="12">
         <v>8.2915296108330393E-3</v>
       </c>
     </row>
@@ -1885,10 +1884,10 @@
         <v>64</v>
       </c>
       <c r="D3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E3" t="s">
         <v>69</v>
-      </c>
-      <c r="E3" t="s">
-        <v>70</v>
       </c>
       <c r="F3" t="s">
         <v>62</v>
@@ -1896,13 +1895,13 @@
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B4" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="6">
         <v>-0.22076642774196101</v>
       </c>
-      <c r="E4" s="11">
+      <c r="E4" s="10">
         <v>-0.203504529529107</v>
       </c>
       <c r="F4" s="7">
@@ -1913,13 +1912,13 @@
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B5" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="6">
         <v>-0.22076642774196101</v>
       </c>
-      <c r="E5" s="11">
+      <c r="E5" s="10">
         <v>-0.20845554762353399</v>
       </c>
       <c r="F5" s="7">
@@ -1930,13 +1929,13 @@
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B6" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="6">
         <v>-0.22076642774196101</v>
       </c>
-      <c r="E6" s="11">
+      <c r="E6" s="10">
         <v>-0.20474965314377999</v>
       </c>
       <c r="F6" s="7">
@@ -1946,14 +1945,14 @@
       <c r="G6" s="4"/>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="6" t="s">
         <v>61</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="6">
         <v>-0.22076642774196101</v>
       </c>
-      <c r="E7" s="11">
+      <c r="E7" s="10">
         <v>-0.19502774912589299</v>
       </c>
       <c r="F7" s="7">
@@ -1962,14 +1961,14 @@
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B8" s="10" t="s">
-        <v>73</v>
+      <c r="B8" s="6" t="s">
+        <v>72</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6">
         <v>-0.22076642774196101</v>
       </c>
-      <c r="E8" s="11">
+      <c r="E8" s="10">
         <v>-0.19504492079197</v>
       </c>
       <c r="F8" s="7">

</xml_diff>